<commit_message>
working on new dictionary page, map generation code, and editing pollinator-smart content
</commit_message>
<xml_diff>
--- a/database/static/Data Definitions_public_03112025.xlsx
+++ b/database/static/Data Definitions_public_03112025.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myuva-my.sharepoint.com/personal/emm2t_virginia_edu/Documents/Solar Database/Solar Data Misc/Website Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/WorkDragon/Documents/WeldonCooper/SolarDatabase/solar-database/database/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F8C2B4-979B-46AA-A1AA-895FBC3A9F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D544C4-75EE-8148-9CFB-4962229A3484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F7BCD3F9-5FE9-4ACA-9E3A-4C83CABA7A20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F7BCD3F9-5FE9-4ACA-9E3A-4C83CABA7A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Definitions 031125" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Definitions 031125'!$A$4:$D$4</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -236,9 +239,6 @@
     <t>Local application documents (meeting minutes)</t>
   </si>
   <si>
-    <t>Date(s)- Local Permit Amendment</t>
-  </si>
-  <si>
     <t>local_permit_amend_date</t>
   </si>
   <si>
@@ -296,9 +296,6 @@
     <t xml:space="preserve">Permit tracking number assigned by DEQ </t>
   </si>
   <si>
-    <t xml:space="preserve">DEQ Renewable Energy Project Status: https://www.deq.virginia.gov/permits/renewable-energy/renewable-energy-project-status </t>
-  </si>
-  <si>
     <t>SCC Certificate Number</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
   </si>
   <si>
     <t xml:space="preserve">This datatpoint captures whether the project is officially enrolled in Dominion's shared solar program (MW have been allotted to subscriber organization.) </t>
-  </si>
-  <si>
-    <t>Dominon Shared Solar Program : https://www.dominionenergy.com/virginia/renewable-energy-programs/shared-solar-program</t>
   </si>
   <si>
     <t>Mined Land</t>
@@ -358,6 +352,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">For certified projects, "stage of development" describes the milestone of development certified, based on program defintions and DCR records. Certification for each milestone is a separate and unique achievement. There are six milestone certifications:  </t>
     </r>
@@ -367,6 +362,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>"Design"</t>
     </r>
@@ -375,6 +371,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>- the project is either pre-construction or less than 2 years old, the Pollinator-Smart Committee has concurred that the design meets the criteria for Pollinator-Smart. The site plan design including the planting plan (vegetation management plan) meets Pollinator Smart Certification per the proposed or retrofit solar sites scorecard version 2.0a (the blue form). "</t>
     </r>
@@ -384,6 +381,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Monitoring Year 2, Monitoring Year 4, Monitoring Year 6, or Monitoring Year 8</t>
     </r>
@@ -392,6 +390,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>"- The year indicates how many years since vegetation has been established. The project has been monitored and assessed with the Monitoring Scorecard version 2.0b (the green form). The Pollinator-Smart Committee concurs that the vegetation on the ground meets the requirement for Pollinator Smart based on review of the scorecard and Monitoring Report.  "</t>
     </r>
@@ -401,6 +400,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Lifetime</t>
     </r>
@@ -409,6 +409,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">"- The site has been certified at all past milestones and has developed a long term mangement plan. The plan, Year 10 monitoring , and scorecard have been reviewed by the Pollinator Smart committee and they concur with the assessment.  </t>
     </r>
@@ -474,9 +475,6 @@
     <t>Queue number assigned by PJM; matched to local project by UVA based on best available information.</t>
   </si>
   <si>
-    <t>PJM Queue, Serial Service Request: https://www.pjm.com/planning/service-requests/serial-service-request-status</t>
-  </si>
-  <si>
     <t>EIA- Plant ID</t>
   </si>
   <si>
@@ -505,13 +503,25 @@
   </si>
   <si>
     <t>Detailed project development status according to the EIA. See EIA for their definitions.</t>
+  </si>
+  <si>
+    <t>DEQ Renewable Energy Project Status</t>
+  </si>
+  <si>
+    <t>PJM Queue, Serial Service Request</t>
+  </si>
+  <si>
+    <t>Dominon Shared Solar Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,17 +539,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -613,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -644,6 +657,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,19 +997,19 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C22"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="46.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
-    <col min="4" max="4" width="75.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="75.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1001,19 +1017,19 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1027,707 +1043,712 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="91.5">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45.75">
-      <c r="A24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="60.75">
-      <c r="A29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="120">
-      <c r="A30" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="321">
-      <c r="A31" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="137.25">
-      <c r="A32" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="121.5">
-      <c r="A33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:D4" xr:uid="{AFB4161F-F0BF-4CEC-AA45-3B2EB98ACFBB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D39">
+      <sortCondition ref="A4:A39"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>